<commit_message>
add colume header condition and login with mulitple data
</commit_message>
<xml_diff>
--- a/src/test/java/com/testData/TestData.xlsx
+++ b/src/test/java/com/testData/TestData.xlsx
@@ -16,21 +16,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Selenium</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Sankar</t>
   </si>
   <si>
-    <t>protractor</t>
-  </si>
-  <si>
     <t>Naman</t>
   </si>
   <si>
-    <t>Murari</t>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>buy</t>
   </si>
 </sst>
 </file>
@@ -365,33 +368,36 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>123</v>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>